<commit_message>
add atmos for cmip6_cmcc_cmcc-cm2-sr5_atmos
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-cm2-sr5/cmip6_cmcc_cmcc-cm2-sr5_atmos.xlsx
+++ b/cmip6/models/cmcc-cm2-sr5/cmip6_cmcc_cmcc-cm2-sr5_atmos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/models/cmcc-cm2-sr5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634CB5F2-F288-7C47-9FF4-FBCF62601015}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B7BFAB-E2CB-3A47-B95B-C54CFC26F9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="460" windowWidth="20580" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5020" yWindow="460" windowWidth="20580" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1721" uniqueCount="1140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="1141">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -3458,6 +3458,9 @@
   </si>
   <si>
     <t>Tomas Lovato</t>
+  </si>
+  <si>
+    <t>NAVARRA-ANTONIO</t>
   </si>
 </sst>
 </file>
@@ -5734,10 +5737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5800,47 +5803,47 @@
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>1089</v>
+        <v>1140</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>1090</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="9" t="s">
+    <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>1089</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>1091</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>42</v>
@@ -5848,7 +5851,7 @@
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>42</v>
@@ -5856,23 +5859,23 @@
     </row>
     <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>158</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>218</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>218</v>
@@ -5880,15 +5883,15 @@
     </row>
     <row r="25" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>368</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>368</v>
@@ -5896,7 +5899,7 @@
     </row>
     <row r="27" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>368</v>
@@ -5904,15 +5907,15 @@
     </row>
     <row r="28" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>614</v>
+        <v>368</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>614</v>
@@ -5920,7 +5923,7 @@
     </row>
     <row r="30" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>614</v>
@@ -5928,7 +5931,7 @@
     </row>
     <row r="31" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>614</v>
@@ -5936,7 +5939,7 @@
     </row>
     <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>614</v>
@@ -5944,7 +5947,7 @@
     </row>
     <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>614</v>
@@ -5952,15 +5955,15 @@
     </row>
     <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>715</v>
+        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>715</v>
@@ -5968,7 +5971,7 @@
     </row>
     <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B36" s="11" t="s">
         <v>715</v>
@@ -5976,23 +5979,23 @@
     </row>
     <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>755</v>
+        <v>715</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>926</v>
+        <v>755</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>926</v>
@@ -6000,7 +6003,7 @@
     </row>
     <row r="40" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="B40" s="11" t="s">
         <v>926</v>
@@ -6008,7 +6011,7 @@
     </row>
     <row r="41" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="B41" s="11" t="s">
         <v>926</v>
@@ -6016,24 +6019,32 @@
     </row>
     <row r="42" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>926</v>
       </c>
     </row>
+    <row r="43" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>926</v>
+      </c>
+    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B11" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B12" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:B42" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20:B43" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Grid,Dynamical Core,Radiation,Turbulence Convection,Microphysics Precipitation,Cloud Scheme,Observation Simulation,Gravity Waves,Natural Forcing"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A15" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A16" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>